<commit_message>
Fix typos in timesheet
</commit_message>
<xml_diff>
--- a/Marcin Kuchta Praktyki Timesheet.xlsx
+++ b/Marcin Kuchta Praktyki Timesheet.xlsx
@@ -102,9 +102,6 @@
     <t>Projekt - AWS - rejestracja, czytanie dokumentacji, planowanie struktury projektu  (AWS Amplify, Lambda, API Gateway)</t>
   </si>
   <si>
-    <t>Projekt - AWS - stworzenie API Gaterway i  Lambdy, konfiguracja i połączenie ich ze sobą</t>
-  </si>
-  <si>
     <t>Projekt - komunikacja klient -&gt; Lambda, scrapowanie lambdą po wybranym zdaniu, sprzątanie niepotrzebnych zależności, testowych zmiennych, wprowadzenie zmiennych środowiskowych dla AWS Amplify</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Projekt - dodanie scrapowania daty z każdej ze stron, sortowanie artykułów od najnowszego do najstarszego, przycisk zmieniający kierunek sortowania, czytanie na temat wywoływania kolejnych Lambd z jednej w celu przyśpieszenia działania strony w przyszłości</t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt - czytanie dokumentacji AWS Lambda, rozbijanie jednej lamby na mniejsze - wywoływane przez jedną, agregującą dane, parugodzinna walka z bugiem spodowanym nieścisłościami w dokumentacji </t>
-  </si>
-  <si>
     <t>Projekt - dokończenie podziału na lambdę główną i jej dzieci, przepisanie funkcji scrapujących - każda jako osobna Lambda (zmiana nie przyśpieszyła znacznie wyszukiwania przez problemy ze zwracaniem danych z asynchronicznych Lambd , jednak zmnieszyła niemal 9-krotnie rozmiar plików przechowywanych na serwerach AWS)</t>
   </si>
   <si>
@@ -159,10 +153,16 @@
     <t xml:space="preserve">Projekt - całkowite dodanie zapisywania artykułów na poźniej w local storage, zmiana nazwy komponentu Sort na bardziej pasującą po dodaniu do niego przycisku pokazującego zapisane artykuły (HeaderButtons), dodanie wyświetlania zapisanych artukułów </t>
   </si>
   <si>
-    <t>Projekt - praca nad przepisaniem apki w taki sposób, aby ostatnie pobrane artykuły były zapisane w session storage, jednak zdecydował się nie implementować tego w końcowym produkcie - spowalnia działanie strony i wprowadza niepotrzebne zamieszanie</t>
-  </si>
-  <si>
     <t>Projekt  - poprawa warunków wyświetlania przycisków, napis z ilością zapisanych artykułów, pozbycie się stanu savedArticles, który okazał sie zbędny po odpowiednich zmianach w kodzie, naprawa błedu przy usuwania zapisanych artkułów, naprawa pobierania daty ze stron (czasem daty różniły sie o jeden dzień), poprawne sortowanie według daty (wcześniej artykuły z dziennik.pl były ustawiane wyżej niż reszta, ponieważ jako jedyne miały podaną godzinę utworzenia), dodanie możliwości wymuszenia wyszukiwania naciskając enter na formie</t>
+  </si>
+  <si>
+    <t>Projekt - AWS - stworzenie API Gateway i  Lambdy, konfiguracja i połączenie ich ze sobą</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projekt - czytanie dokumentacji AWS Lambda, rozbijanie jednej lambdy na mniejsze - wywoływane przez jedną, agregującą dane, parugodzinna walka z bugiem spodowanym nieścisłościami w dokumentacji </t>
+  </si>
+  <si>
+    <t>Projekt - praca nad przepisaniem apki w taki sposób, aby ostatnie pobrane artykuły były zapisane w session storage, jednak zdecydowałem się nie implementować tego w końcowym produkcie - spowalnia działanie strony i wprowadza niepotrzebne zamieszanie</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
         <v>6.5</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>5.5</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>5.5</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>8.5</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>5.5</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>4.5</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1270,6 +1270,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FFFA20196C5244A198B956263BCCC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e665c9909af2d00025ac938ed956f4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65d88d86-0354-4735-9d62-80a4ac60412a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d6152cd73a56170a76ea3621d94087c" ns2:_="">
     <xsd:import namespace="65d88d86-0354-4735-9d62-80a4ac60412a"/>
@@ -1401,22 +1416,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCBFDAD8-0F07-4DA1-82D3-259155DCA012}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1432,21 +1449,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE0AA63-4C71-4853-AA83-FB6609B135DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A3B923-F919-4A22-94D3-DBAAFD20A330}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>